<commit_message>
getting spreadsheets to run
</commit_message>
<xml_diff>
--- a/projects/DC_analysis/PTool_1_of_5.xlsx
+++ b/projects/DC_analysis/PTool_1_of_5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="493">
   <si>
     <t>type</t>
   </si>
@@ -5754,7 +5754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6190,9 +6190,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z135"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8:B21"/>
+      <selection pane="bottomLeft" activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6527,6 +6527,9 @@
       <c r="P9" s="30" t="s">
         <v>263</v>
       </c>
+      <c r="R9" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="10" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="b">
@@ -6593,6 +6596,9 @@
         <v>263</v>
       </c>
       <c r="Q11" s="3"/>
+      <c r="R11" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="12" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="b">
@@ -6650,6 +6656,9 @@
       <c r="P13" s="30" t="s">
         <v>263</v>
       </c>
+      <c r="R13" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="14" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="b">
@@ -6708,7 +6717,9 @@
         <v>263</v>
       </c>
       <c r="Q15" s="37"/>
-      <c r="R15" s="2"/>
+      <c r="R15" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="16" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="b">
@@ -6772,6 +6783,9 @@
       <c r="P17" s="30" t="s">
         <v>263</v>
       </c>
+      <c r="R17" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="18" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="b">
@@ -6828,6 +6842,9 @@
       </c>
       <c r="P19" s="30" t="s">
         <v>263</v>
+      </c>
+      <c r="R19" s="30" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -6895,6 +6912,9 @@
         <v>263</v>
       </c>
       <c r="Q21" s="3"/>
+      <c r="R21" s="30" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I22" s="30"/>

</xml_diff>